<commit_message>
A punto de terminar proyecto
</commit_message>
<xml_diff>
--- a/TRAND3.xlsx
+++ b/TRAND3.xlsx
@@ -2,23 +2,34 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zullo\OneDrive\Escritorio\IV - Semestre\Lenguajes y Automatas I\UIV\Lexico_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA1F290-26B0-4699-80DD-E8A0BC611296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7141E1E7-4AC9-41CE-9E72-9E777DCF97AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF48CD0A-8B25-45AB-8C98-1056E4011020}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0B55FBFE-415A-4501-9873-421BD18FE1C4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -41,7 +52,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -49,7 +60,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -57,13 +68,13 @@
       <b/>
       <sz val="11"/>
       <color theme="9"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -72,7 +83,7 @@
       <u/>
       <sz val="11"/>
       <color theme="9"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -97,8 +108,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -113,6 +133,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -132,9 +155,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,39 +165,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -226,7 +249,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -278,7 +301,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -337,13 +360,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -352,6 +368,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -416,28 +439,45 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E074FEF-8AC6-4A79-9DD9-98018E896E09}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27552F2-8742-4294-B48A-0D8C8D469A6B}">
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="S19" workbookViewId="0">
+      <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="9.109375" style="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
@@ -447,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1">
         <v>33</v>
@@ -520,7 +560,7 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -2040,1447 +2080,1446 @@
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P21" s="4">
+      <c r="A21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21" s="7">
         <v>19</v>
       </c>
-      <c r="Q21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="3" t="s">
+      <c r="Q21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L22" s="4">
+      <c r="A22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="7">
         <v>22</v>
       </c>
-      <c r="M22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="3" t="s">
+      <c r="M22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P23" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="3" t="s">
+      <c r="A23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L24" s="4">
+      <c r="A24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="7">
         <v>24</v>
       </c>
-      <c r="M24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="3" t="s">
+      <c r="M24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="3" t="s">
+      <c r="A25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L26" s="1">
+      <c r="A26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" s="4">
         <v>24</v>
       </c>
-      <c r="M26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="3" t="s">
+      <c r="M26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L27" s="1">
+      <c r="A27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="4">
         <v>24</v>
       </c>
-      <c r="M27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S27" s="1">
+      <c r="M27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S27" s="4">
         <v>24</v>
       </c>
-      <c r="T27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="3" t="s">
+      <c r="T27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="4">
         <v>27</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="4">
         <v>27</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="4">
         <v>27</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="4">
         <v>27</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="4">
         <v>27</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="4">
         <v>27</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="4">
         <v>27</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="4">
         <v>27</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28" s="4">
         <v>27</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28" s="4">
         <v>27</v>
       </c>
-      <c r="L28" s="1">
+      <c r="L28" s="4">
         <v>27</v>
       </c>
-      <c r="M28" s="1">
+      <c r="M28" s="4">
         <v>27</v>
       </c>
-      <c r="N28" s="1">
+      <c r="N28" s="4">
         <v>27</v>
       </c>
-      <c r="O28" s="1">
+      <c r="O28" s="4">
         <v>27</v>
       </c>
-      <c r="P28" s="1">
+      <c r="P28" s="4">
         <v>27</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="Q28" s="4">
         <v>27</v>
       </c>
-      <c r="R28" s="1">
+      <c r="R28" s="4">
         <v>27</v>
       </c>
-      <c r="S28" s="1">
+      <c r="S28" s="4">
         <v>27</v>
       </c>
-      <c r="T28" s="1">
+      <c r="T28" s="4">
         <v>28</v>
       </c>
-      <c r="U28" s="1">
+      <c r="U28" s="4">
         <v>27</v>
       </c>
-      <c r="V28" s="1">
+      <c r="V28" s="4">
         <v>27</v>
       </c>
-      <c r="W28" s="1">
+      <c r="W28" s="4">
         <v>27</v>
       </c>
-      <c r="X28" s="1">
+      <c r="X28" s="4">
         <v>27</v>
       </c>
-      <c r="Y28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z28" s="1">
+      <c r="Y28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="4">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P29" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z29" s="3" t="s">
+      <c r="A29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+      <c r="A30" s="4">
         <v>30</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="4">
         <v>30</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="4">
         <v>30</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="4">
         <v>30</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="4">
         <v>30</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="4">
         <v>30</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="4">
         <v>30</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="4">
         <v>30</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="4">
         <v>30</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30" s="4">
         <v>30</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="4">
         <v>30</v>
       </c>
-      <c r="L30" s="1">
+      <c r="L30" s="4">
         <v>30</v>
       </c>
-      <c r="M30" s="1">
+      <c r="M30" s="4">
         <v>30</v>
       </c>
-      <c r="N30" s="1">
+      <c r="N30" s="4">
         <v>30</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O30" s="4">
         <v>30</v>
       </c>
-      <c r="P30" s="1">
+      <c r="P30" s="4">
         <v>30</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="Q30" s="4">
         <v>30</v>
       </c>
-      <c r="R30" s="1">
+      <c r="R30" s="4">
         <v>30</v>
       </c>
-      <c r="S30" s="1">
+      <c r="S30" s="4">
         <v>30</v>
       </c>
-      <c r="T30" s="1">
+      <c r="T30" s="4">
         <v>30</v>
       </c>
-      <c r="U30" s="1">
+      <c r="U30" s="4">
         <v>30</v>
       </c>
-      <c r="V30" s="1">
+      <c r="V30" s="4">
         <v>30</v>
       </c>
-      <c r="W30" s="1">
+      <c r="W30" s="4">
         <v>30</v>
       </c>
-      <c r="X30" s="1">
+      <c r="X30" s="4">
         <v>30</v>
       </c>
-      <c r="Y30" s="1">
+      <c r="Y30" s="4">
         <v>30</v>
       </c>
-      <c r="Z30" s="1">
+      <c r="Z30" s="4">
         <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="U31" s="1">
+      <c r="A31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="S31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U31" s="4">
         <v>31</v>
       </c>
-      <c r="V31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="W31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="X31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z31" s="2" t="s">
+      <c r="V31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="W31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P32" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z32" s="3" t="s">
+      <c r="A32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P32" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="A33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4">
         <v>32</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P33" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="3" t="s">
+      <c r="D33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P33" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P34" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="3" t="s">
+      <c r="A34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P34" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L35" s="1">
+      <c r="A35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L35" s="4">
         <v>17</v>
       </c>
-      <c r="M35" s="1">
-        <v>36</v>
-      </c>
-      <c r="N35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P35" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W35" s="1">
+      <c r="M35" s="4">
+        <v>36</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P35" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W35" s="4">
         <v>35</v>
       </c>
-      <c r="X35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z35" s="3" t="s">
+      <c r="X35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+      <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="4">
         <v>35</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="4">
         <v>35</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="4">
         <v>35</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="4">
         <v>35</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="4">
         <v>35</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="4">
         <v>35</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36" s="4">
         <v>35</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36" s="4">
         <v>35</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J36" s="4">
         <v>35</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="4">
         <v>35</v>
       </c>
-      <c r="L36" s="1">
+      <c r="L36" s="4">
         <v>35</v>
       </c>
-      <c r="M36" s="1">
+      <c r="M36" s="4">
         <v>35</v>
       </c>
-      <c r="N36" s="1">
+      <c r="N36" s="4">
         <v>35</v>
       </c>
-      <c r="O36" s="1">
+      <c r="O36" s="4">
         <v>35</v>
       </c>
-      <c r="P36" s="1">
+      <c r="P36" s="4">
         <v>35</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="Q36" s="4">
         <v>35</v>
       </c>
-      <c r="R36" s="1">
+      <c r="R36" s="4">
         <v>35</v>
       </c>
-      <c r="S36" s="1">
+      <c r="S36" s="4">
         <v>35</v>
       </c>
-      <c r="T36" s="1">
+      <c r="T36" s="4">
         <v>35</v>
       </c>
-      <c r="U36" s="1">
+      <c r="U36" s="4">
         <v>35</v>
       </c>
-      <c r="V36" s="1">
+      <c r="V36" s="4">
         <v>35</v>
       </c>
-      <c r="W36" s="1">
+      <c r="W36" s="4">
         <v>35</v>
       </c>
-      <c r="X36" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="1">
+      <c r="X36" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="4">
         <v>35</v>
       </c>
-      <c r="Z36" s="1">
+      <c r="Z36" s="4">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1">
-        <v>36</v>
-      </c>
-      <c r="C37" s="1">
-        <v>36</v>
-      </c>
-      <c r="D37" s="1">
-        <v>36</v>
-      </c>
-      <c r="E37" s="1">
-        <v>36</v>
-      </c>
-      <c r="F37" s="1">
-        <v>36</v>
-      </c>
-      <c r="G37" s="1">
-        <v>36</v>
-      </c>
-      <c r="H37" s="1">
-        <v>36</v>
-      </c>
-      <c r="I37" s="1">
-        <v>36</v>
-      </c>
-      <c r="J37" s="1">
-        <v>36</v>
-      </c>
-      <c r="K37" s="1">
-        <v>36</v>
-      </c>
-      <c r="L37" s="1">
-        <v>36</v>
-      </c>
-      <c r="M37" s="1">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4">
+        <v>36</v>
+      </c>
+      <c r="C37" s="4">
+        <v>36</v>
+      </c>
+      <c r="D37" s="4">
+        <v>36</v>
+      </c>
+      <c r="E37" s="4">
+        <v>36</v>
+      </c>
+      <c r="F37" s="4">
+        <v>36</v>
+      </c>
+      <c r="G37" s="4">
+        <v>36</v>
+      </c>
+      <c r="H37" s="4">
+        <v>36</v>
+      </c>
+      <c r="I37" s="4">
+        <v>36</v>
+      </c>
+      <c r="J37" s="4">
+        <v>36</v>
+      </c>
+      <c r="K37" s="4">
+        <v>36</v>
+      </c>
+      <c r="L37" s="4">
+        <v>36</v>
+      </c>
+      <c r="M37" s="4">
         <v>37</v>
       </c>
-      <c r="N37" s="1">
-        <v>36</v>
-      </c>
-      <c r="O37" s="1">
-        <v>36</v>
-      </c>
-      <c r="P37" s="1">
-        <v>36</v>
-      </c>
-      <c r="Q37" s="1">
-        <v>36</v>
-      </c>
-      <c r="R37" s="1">
-        <v>36</v>
-      </c>
-      <c r="S37" s="1">
-        <v>36</v>
-      </c>
-      <c r="T37" s="1">
-        <v>36</v>
-      </c>
-      <c r="U37" s="1">
-        <v>36</v>
-      </c>
-      <c r="V37" s="1">
-        <v>36</v>
-      </c>
-      <c r="W37" s="1">
-        <v>36</v>
-      </c>
-      <c r="X37" s="1">
-        <v>36</v>
-      </c>
-      <c r="Y37" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z37" s="1">
+      <c r="N37" s="4">
+        <v>36</v>
+      </c>
+      <c r="O37" s="4">
+        <v>36</v>
+      </c>
+      <c r="P37" s="4">
+        <v>36</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>36</v>
+      </c>
+      <c r="R37" s="4">
+        <v>36</v>
+      </c>
+      <c r="S37" s="4">
+        <v>36</v>
+      </c>
+      <c r="T37" s="4">
+        <v>36</v>
+      </c>
+      <c r="U37" s="4">
+        <v>36</v>
+      </c>
+      <c r="V37" s="4">
+        <v>36</v>
+      </c>
+      <c r="W37" s="4">
+        <v>36</v>
+      </c>
+      <c r="X37" s="4">
+        <v>36</v>
+      </c>
+      <c r="Y37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="4">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
-      <c r="B38" s="1">
-        <v>36</v>
-      </c>
-      <c r="C38" s="1">
-        <v>36</v>
-      </c>
-      <c r="D38" s="1">
-        <v>36</v>
-      </c>
-      <c r="E38" s="1">
-        <v>36</v>
-      </c>
-      <c r="F38" s="1">
-        <v>36</v>
-      </c>
-      <c r="G38" s="1">
-        <v>36</v>
-      </c>
-      <c r="H38" s="1">
-        <v>36</v>
-      </c>
-      <c r="I38" s="1">
-        <v>36</v>
-      </c>
-      <c r="J38" s="1">
-        <v>36</v>
-      </c>
-      <c r="K38" s="1">
-        <v>36</v>
-      </c>
-      <c r="L38" s="1">
-        <v>36</v>
-      </c>
-      <c r="M38" s="1">
+      <c r="A38" s="4">
+        <v>36</v>
+      </c>
+      <c r="B38" s="4">
+        <v>36</v>
+      </c>
+      <c r="C38" s="4">
+        <v>36</v>
+      </c>
+      <c r="D38" s="4">
+        <v>36</v>
+      </c>
+      <c r="E38" s="4">
+        <v>36</v>
+      </c>
+      <c r="F38" s="4">
+        <v>36</v>
+      </c>
+      <c r="G38" s="4">
+        <v>36</v>
+      </c>
+      <c r="H38" s="4">
+        <v>36</v>
+      </c>
+      <c r="I38" s="4">
+        <v>36</v>
+      </c>
+      <c r="J38" s="4">
+        <v>36</v>
+      </c>
+      <c r="K38" s="4">
+        <v>36</v>
+      </c>
+      <c r="L38" s="4">
+        <v>36</v>
+      </c>
+      <c r="M38" s="4">
         <v>37</v>
       </c>
-      <c r="N38" s="1">
-        <v>36</v>
-      </c>
-      <c r="O38" s="1">
-        <v>36</v>
-      </c>
-      <c r="P38" s="1">
-        <v>36</v>
-      </c>
-      <c r="Q38" s="1">
-        <v>36</v>
-      </c>
-      <c r="R38" s="1">
-        <v>36</v>
-      </c>
-      <c r="S38" s="1">
-        <v>36</v>
-      </c>
-      <c r="T38" s="1">
-        <v>36</v>
-      </c>
-      <c r="U38" s="1">
-        <v>36</v>
-      </c>
-      <c r="V38" s="1">
-        <v>36</v>
-      </c>
-      <c r="W38" s="1">
-        <v>0</v>
-      </c>
-      <c r="X38" s="1">
-        <v>36</v>
-      </c>
-      <c r="Y38" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z38" s="1">
+      <c r="N38" s="4">
+        <v>36</v>
+      </c>
+      <c r="O38" s="4">
+        <v>36</v>
+      </c>
+      <c r="P38" s="4">
+        <v>36</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>36</v>
+      </c>
+      <c r="R38" s="4">
+        <v>36</v>
+      </c>
+      <c r="S38" s="4">
+        <v>36</v>
+      </c>
+      <c r="T38" s="4">
+        <v>36</v>
+      </c>
+      <c r="U38" s="4">
+        <v>36</v>
+      </c>
+      <c r="V38" s="4">
+        <v>36</v>
+      </c>
+      <c r="W38" s="4">
+        <v>0</v>
+      </c>
+      <c r="X38" s="4">
+        <v>36</v>
+      </c>
+      <c r="Y38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="4">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>